<commit_message>
update new calculation process
</commit_message>
<xml_diff>
--- a/parameters_dataframe.xlsx
+++ b/parameters_dataframe.xlsx
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="新細明體"/>
       <family val="2"/>
@@ -42,11 +42,6 @@
       <family val="3"/>
       <sz val="9"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
       <name val="新細明體"/>
@@ -115,22 +110,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -498,10 +487,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -571,41 +560,41 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>I230815001</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>54000</v>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>PB1-2307000305</t>
+        <v>8000</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>P0091240100179</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.0051</v>
+        <v>0.616</v>
       </c>
       <c r="H2" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="I2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="n">
         <v>45364</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -615,41 +604,41 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>I230815001</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>26000</v>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>PB1-2307000305</t>
+        <v>8000</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>P0091240100179</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.0051</v>
+        <v>0.616</v>
       </c>
       <c r="H3" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="I3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="n">
         <v>45364</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -659,41 +648,41 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>I230815001</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3DSGS1G4000SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>M4G</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>15000</v>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>PB1-2307000305</t>
+        <v>8000</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>P0091240200042</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.007900000000000001</v>
+        <v>0.616</v>
       </c>
       <c r="H4" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="I4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="n">
         <v>45364</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -703,41 +692,41 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>I230815001</t>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MBRD5100G-L10</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3DYMBRD5100SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MBRD5100</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5000</v>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>PB1-2307000305</t>
+        <v>9000</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>P0091231200126</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.1067</v>
+        <v>1.3</v>
       </c>
       <c r="H5" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="I5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="n">
         <v>45364</v>
       </c>
       <c r="J5" t="inlineStr">
@@ -747,41 +736,41 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>I230815001</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3DZ013W505S0B02</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6000</v>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>PB1-2111000268</t>
+        <v>48000</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>P0091231200081</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.007</v>
+        <v>1.3</v>
       </c>
       <c r="H6" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="I6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="n">
         <v>45364</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -791,41 +780,41 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>I230815001</t>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P2SD75AG-730</t>
+          <t>PS5020KN-Cu-L10</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3DT075200U0SB01</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>P2SD75AG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5000</v>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>PB1-2308000138</t>
+        <v>3000</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>P0091240100063</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.0344</v>
+        <v>0.63</v>
       </c>
       <c r="H7" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="I7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="n">
         <v>45364</v>
       </c>
       <c r="J7" t="inlineStr">
@@ -835,41 +824,41 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>I230815001</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P4SMAJ64AG-L10</t>
+          <t>PS5020KN-Cu-L10</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3DT064400U0SB03</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>P4SMAJ64AG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>PB1-2105000582</t>
+        <v>33000</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>P0091240100028</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0.031</v>
+        <v>0.63</v>
       </c>
       <c r="H8" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="I8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="n">
         <v>45364</v>
       </c>
       <c r="J8" t="inlineStr">
@@ -879,13 +868,48 @@
       </c>
     </row>
     <row r="9">
-      <c r="F9" s="2" t="n"/>
-    </row>
-    <row r="10">
-      <c r="F10" s="2" t="n"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="2" t="n"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>IS24031302</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PS5020KN-Cu-L10</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10T3-5019-2R01</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>LS5019NG-T3R</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>P0091240100028</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>45364</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>B0000010-3</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -899,7 +923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -912,19 +936,19 @@
     <col width="16" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
     <col width="22" customWidth="1" min="11" max="11"/>
     <col width="16" customWidth="1" min="12" max="12"/>
-    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
     <col width="8" customWidth="1" min="14" max="14"/>
     <col width="15" customWidth="1" min="15" max="15"/>
     <col width="14" customWidth="1" min="16" max="16"/>
-    <col width="16" customWidth="1" min="17" max="17"/>
-    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="14" customWidth="1" min="17" max="17"/>
+    <col width="9" customWidth="1" min="18" max="18"/>
     <col width="12" customWidth="1" min="19" max="19"/>
     <col width="10" customWidth="1" min="20" max="20"/>
     <col width="22" customWidth="1" min="21" max="21"/>
@@ -937,7 +961,7 @@
     <col width="9" customWidth="1" min="28" max="28"/>
     <col width="7" customWidth="1" min="29" max="29"/>
     <col width="11" customWidth="1" min="30" max="30"/>
-    <col width="42" customWidth="1" min="31" max="31"/>
+    <col width="18" customWidth="1" min="31" max="31"/>
     <col width="10" customWidth="1" min="32" max="32"/>
     <col width="6" customWidth="1" min="33" max="33"/>
     <col width="8" customWidth="1" min="34" max="34"/>
@@ -946,182 +970,182 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>delivery_date</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>invoice_series</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>purchase_order</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>customer_no</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>customer_name</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>lot</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>part_number</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>DC</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>date_code</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>customer_part_number</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>product_number</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>new_lot</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>new_DC</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>new_date_code</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>new_quantity</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>marking_code</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>package</t>
         </is>
       </c>
-      <c r="S1" s="5" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>unit_price</t>
         </is>
       </c>
-      <c r="T1" s="5" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>currency</t>
         </is>
       </c>
-      <c r="U1" s="5" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>small_label_quantity</t>
         </is>
       </c>
-      <c r="V1" s="5" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>small_label_copies</t>
         </is>
       </c>
-      <c r="W1" s="5" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>medium_label_quantity</t>
         </is>
       </c>
-      <c r="X1" s="5" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>medium_label_copies</t>
         </is>
       </c>
-      <c r="Y1" s="5" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>large_label_quantity</t>
         </is>
       </c>
-      <c r="Z1" s="5" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>large_label_copies</t>
         </is>
       </c>
-      <c r="AA1" s="5" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>out_date</t>
         </is>
       </c>
-      <c r="AB1" s="5" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>expired</t>
         </is>
       </c>
-      <c r="AC1" s="5" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>store</t>
         </is>
       </c>
-      <c r="AD1" s="5" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>row_index</t>
         </is>
       </c>
-      <c r="AE1" s="5" t="inlineStr">
+      <c r="AE1" s="4" t="inlineStr">
         <is>
           <t>remark</t>
         </is>
       </c>
-      <c r="AF1" s="5" t="inlineStr">
+      <c r="AF1" s="4" t="inlineStr">
         <is>
           <t>sampling</t>
         </is>
       </c>
-      <c r="AG1" s="5" t="inlineStr">
+      <c r="AG1" s="4" t="inlineStr">
         <is>
           <t>MPQ</t>
         </is>
       </c>
-      <c r="AH1" s="5" t="inlineStr">
+      <c r="AH1" s="4" t="inlineStr">
         <is>
           <t>deduct</t>
         </is>
       </c>
-      <c r="AI1" s="5" t="inlineStr">
+      <c r="AI1" s="4" t="inlineStr">
         <is>
           <t>month</t>
         </is>
       </c>
-      <c r="AJ1" s="5" t="inlineStr">
+      <c r="AJ1" s="4" t="inlineStr">
         <is>
           <t>day</t>
         </is>
@@ -1135,12 +1159,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091240100179</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1155,112 +1179,114 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
+          <t>F210720012AE</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>2315</v>
+        <v>2146</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2023/04/09</t>
+          <t>2021/11/07</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>3000</v>
+        <v>16000</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
-        <v>2315</v>
+          <t>F210720012AEB</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>2346</t>
+        </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2023/04/09</t>
+          <t>2023/11/07</t>
         </is>
       </c>
       <c r="P2" t="n">
-        <v>3000</v>
+        <v>16000</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>SOD123</t>
+          <t>SOD523</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>0.0051</v>
+        <v>0.616</v>
       </c>
       <c r="T2" t="n">
-        <v>31.64</v>
+        <v>1</v>
       </c>
       <c r="U2" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="V2" t="n">
+        <v>2</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>[16000, 16000, 60000]</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>[1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>[16000, 16000, 240000]</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>[1, 2, 0]</t>
+        </is>
+      </c>
+      <c r="AA2" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB2" t="b">
         <v>1</v>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>[3000, 3000, 60000]</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>[3000, 3000, 240000]</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
-        </is>
-      </c>
-      <c r="AA2" t="n">
-        <v>11</v>
-      </c>
-      <c r="AB2" t="b">
-        <v>0</v>
-      </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>Z13</t>
         </is>
       </c>
       <c r="AD2" t="n">
-        <v>6277</v>
+        <v>4060</v>
       </c>
       <c r="AF2" t="n">
-        <v>125</v>
+        <v>315</v>
       </c>
       <c r="AG2" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="AH2" t="b">
         <v>0</v>
@@ -1284,12 +1310,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091240200042</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1304,86 +1330,86 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
+          <t>F22021001106</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>2315</v>
+        <v>2210</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2023/04/09</t>
+          <t>2022/03/06</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>77000</v>
+        <v>8000</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
+          <t>F22021001106</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>2315</v>
+        <v>2210</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2023/04/09</t>
+          <t>2022/03/06</t>
         </is>
       </c>
       <c r="P3" t="n">
-        <v>77000</v>
+        <v>8000</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>SOD123</t>
+          <t>SOD523</t>
         </is>
       </c>
       <c r="S3" t="n">
-        <v>0.0051</v>
+        <v>0.616</v>
       </c>
       <c r="T3" t="n">
-        <v>31.64</v>
+        <v>1</v>
       </c>
       <c r="U3" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="V3" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>[17000, 77000, 60000]</t>
+          <t>[8000, 8000, 60000]</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[1, 1, 0]</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>[77000, 77000, 240000]</t>
+          <t>[8000, 8000, 240000]</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
@@ -1392,24 +1418,24 @@
         </is>
       </c>
       <c r="AA3" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="AB3" t="b">
         <v>0</v>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>暫</t>
         </is>
       </c>
       <c r="AD3" t="n">
-        <v>6281</v>
+        <v>6411</v>
       </c>
       <c r="AF3" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="AG3" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="AH3" t="b">
         <v>0</v>
@@ -1433,12 +1459,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091231200081</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1453,86 +1479,88 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2137</v>
+        <v>2125</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2021/09/05</t>
+          <t>2021/06/13</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>15000</v>
+        <v>48000</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>3DSGS1G4000SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>M4G</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>2137</v>
+          <t>E210430011BYB</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>2325</t>
+        </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2021/09/05</t>
+          <t>2023/06/13</t>
         </is>
       </c>
       <c r="P4" t="n">
-        <v>15000</v>
+        <v>48000</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>SMA</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="S4" t="n">
-        <v>0.007900000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="T4" t="n">
-        <v>31.64</v>
+        <v>1</v>
       </c>
       <c r="U4" t="n">
-        <v>7500</v>
+        <v>3000</v>
       </c>
       <c r="V4" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>[0, 15000, 15000]</t>
+          <t>[48000, 48000, 60000]</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>[0, 1, 1]</t>
+          <t>[1, 1, 0]</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>[15000, 15000, 120000]</t>
+          <t>[48000, 48000, 240000]</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
@@ -1541,24 +1569,24 @@
         </is>
       </c>
       <c r="AA4" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="AB4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>X1</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="AD4" t="n">
-        <v>3090</v>
+        <v>4901</v>
       </c>
       <c r="AF4" t="n">
-        <v>315</v>
+        <v>500</v>
       </c>
       <c r="AG4" t="n">
-        <v>7500</v>
+        <v>3000</v>
       </c>
       <c r="AH4" t="b">
         <v>0</v>
@@ -1582,12 +1610,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091231200126</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1602,77 +1630,78 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>F210813041AC</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>MBRD5100G-L10</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>2148</v>
+        <v>2125</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2021/11/21</t>
+          <t>2021/06/13</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>3DYMBRD5100SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>MBRD5100</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>F210813041AC</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>2148</v>
+          <t>E210430011BYB</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>2325</t>
+        </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>2021/11/21</t>
+          <t>2023/06/13</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>LSYM
-MBRD5100</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>TO252</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="S5" t="n">
-        <v>0.1067</v>
+        <v>1.3</v>
       </c>
       <c r="T5" t="n">
-        <v>31.64</v>
+        <v>1</v>
       </c>
       <c r="U5" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="V5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>[5000, 5000, 50000]</t>
+          <t>[9000, 9000, 60000]</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
@@ -1682,7 +1711,7 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>[5000, 5000, 200000]</t>
+          <t>[9000, 9000, 240000]</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
@@ -1691,31 +1720,24 @@
         </is>
       </c>
       <c r="AA5" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="AB5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="AD5" t="n">
-        <v>3646</v>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>windows user:
-力神料號
-MBRD10100CTG-LS02</t>
-        </is>
+        <v>4901</v>
       </c>
       <c r="AF5" t="n">
         <v>200</v>
       </c>
       <c r="AG5" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="AH5" t="b">
         <v>0</v>
@@ -1739,12 +1761,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PB1-2111000268</t>
+          <t>P0091240100028</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1759,76 +1781,76 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>2239</v>
+        <v>2251</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2022/09/25</t>
+          <t>2022/12/17</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>3DZ013W505S0B02</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>2239</v>
+        <v>2251</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>2022/09/25</t>
+          <t>2022/12/17</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>SOD123</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="S6" t="n">
-        <v>0.007</v>
+        <v>0.63</v>
       </c>
       <c r="T6" t="n">
-        <v>31.64</v>
+        <v>1</v>
       </c>
       <c r="U6" t="n">
         <v>3000</v>
       </c>
       <c r="V6" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>[6000, 6000, 60000]</t>
+          <t>[36000, 36000, 60000]</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
@@ -1838,7 +1860,7 @@
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>[6000, 6000, 240000]</t>
+          <t>[36000, 36000, 240000]</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
@@ -1847,21 +1869,27 @@
         </is>
       </c>
       <c r="AA6" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AB6" t="b">
         <v>0</v>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="AD6" t="n">
-        <v>5363</v>
+        <v>5432</v>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>User:
+BSS138G-T3</t>
+        </is>
       </c>
       <c r="AF6" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="AG6" t="n">
         <v>3000</v>
@@ -1888,12 +1916,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PB1-2308000138</t>
+          <t>P0091240100063</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1908,76 +1936,76 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>P2SD75AG-730</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2325</v>
+        <v>2251</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2023/06/18</t>
+          <t>2022/12/17</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>3DT075200U0SB01</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>P2SD75AG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>2325</v>
+        <v>2251</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>2023/06/18</t>
+          <t>2022/12/17</t>
         </is>
       </c>
       <c r="P7" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>XR</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>SOD123FL</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="S7" t="n">
-        <v>0.0344</v>
+        <v>0.63</v>
       </c>
       <c r="T7" t="n">
-        <v>31.64</v>
+        <v>1</v>
       </c>
       <c r="U7" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="V7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>[5000, 5000, 60000]</t>
+          <t>[3000, 3000, 60000]</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
@@ -1987,7 +2015,7 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>[5000, 5000, 240000]</t>
+          <t>[3000, 3000, 240000]</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
@@ -1996,24 +2024,30 @@
         </is>
       </c>
       <c r="AA7" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="AB7" t="b">
         <v>0</v>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>I2</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="AD7" t="n">
-        <v>6230</v>
+        <v>5432</v>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>User:
+BSS138G-T3</t>
+        </is>
       </c>
       <c r="AF7" t="n">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="AG7" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="AH7" t="b">
         <v>0</v>
@@ -2024,158 +2058,6 @@
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024/03/13</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>I230815001</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>PB1-2105000582</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>B0000010-3</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>協禧微機電</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>F210416513K3</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG-L10</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>2150</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2021/09/26</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>3DT064400U0SB03</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>F210416513K3</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>2150</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>2021/09/26</t>
-        </is>
-      </c>
-      <c r="P8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>LSYM
-RM</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>SMA</t>
-        </is>
-      </c>
-      <c r="S8" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="T8" t="n">
-        <v>31.64</v>
-      </c>
-      <c r="U8" t="n">
-        <v>1800</v>
-      </c>
-      <c r="V8" t="n">
-        <v>2</v>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 25200]</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 100800]</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
-        </is>
-      </c>
-      <c r="AA8" t="n">
-        <v>30</v>
-      </c>
-      <c r="AB8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>A7</t>
-        </is>
-      </c>
-      <c r="AD8" t="n">
-        <v>6086</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>200</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>1800</v>
-      </c>
-      <c r="AH8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="AJ8" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -2192,7 +2074,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2206,65 +2088,65 @@
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="17" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
     <col width="10" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>month</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>day</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>invoice_series</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>purchase_order</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>customer_no</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>customer_name</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>lot</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>part_number</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>DC</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>date_code</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
@@ -2283,12 +2165,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091240100179</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2303,24 +2185,24 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
+          <t>F210720012AE</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2315</v>
+        <v>2146</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2023/04/09</t>
+          <t>2021/11/07</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>3000</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="3">
@@ -2336,12 +2218,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091240200042</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2356,24 +2238,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
+          <t>F22021001106</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2315</v>
+        <v>2210</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2023/04/09</t>
+          <t>2022/03/06</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>77000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="4">
@@ -2389,12 +2271,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091231200081</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2409,24 +2291,24 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2137</v>
+        <v>2125</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2021/09/05</t>
+          <t>2021/06/13</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>15000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="5">
@@ -2442,12 +2324,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091231200126</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -2462,24 +2344,24 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>F210813041AC</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>MBRD5100G-L10</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>2148</v>
+        <v>2125</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2021/11/21</t>
+          <t>2021/06/13</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="6">
@@ -2495,12 +2377,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PB1-2111000268</t>
+          <t>P0091240100028</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -2515,24 +2397,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>2239</v>
+        <v>2251</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2022/09/25</t>
+          <t>2022/12/17</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>6000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="7">
@@ -2548,12 +2430,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PB1-2308000138</t>
+          <t>P0091240100063</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2568,77 +2450,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>P2SD75AG-730</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>2325</v>
+        <v>2251</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2023/06/18</t>
+          <t>2022/12/17</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>I230815001</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>PB1-2105000582</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>B0000010-3</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>協禧微機電</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>F210416513K3</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG-L10</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>2150</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>2021/09/26</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>3600</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
@@ -2652,7 +2481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2664,16 +2493,16 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="6" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="22" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
-    <col width="18" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
     <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="16" customWidth="1" min="14" max="14"/>
+    <col width="14" customWidth="1" min="14" max="14"/>
     <col width="22" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
     <col width="23" customWidth="1" min="17" max="17"/>
@@ -2683,102 +2512,102 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>delivery_date</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>invoice_series</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>customer_no</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>customer_name</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>part_number</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>lot</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>DC</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>customer_part_number</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>product_number</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>new_lot</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>new_DC</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>new_quantity</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>marking_code</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>small_label_quantity</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>small_label_copies</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>medium_label_quantity</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>medium_label_copies</t>
         </is>
       </c>
-      <c r="S1" s="5" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>large_label_quantity</t>
         </is>
       </c>
-      <c r="T1" s="5" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>large_label_copies</t>
         </is>
@@ -2792,7 +2621,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2807,55 +2636,57 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
+          <t>F210720012AE</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2315</v>
+        <v>2146</v>
       </c>
       <c r="H2" t="n">
-        <v>3000</v>
+        <v>16000</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>2315</v>
+          <t>F210720012AEB</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2346</t>
+        </is>
       </c>
       <c r="M2" t="n">
-        <v>3000</v>
+        <v>16000</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>[3000, 3000, 60000]</t>
+          <t>[16000, 16000, 60000]</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -2865,7 +2696,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>[3000, 3000, 240000]</t>
+          <t>[16000, 16000, 240000]</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -2882,7 +2713,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2897,65 +2728,65 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
+          <t>F22021001106</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>2315</v>
+        <v>2210</v>
       </c>
       <c r="H3" t="n">
-        <v>77000</v>
+        <v>8000</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
+          <t>F22021001106</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>2315</v>
+        <v>2210</v>
       </c>
       <c r="M3" t="n">
-        <v>77000</v>
+        <v>8000</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="P3" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>[17000, 77000, 60000]</t>
+          <t>[8000, 8000, 60000]</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[1, 1, 0]</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>[77000, 77000, 240000]</t>
+          <t>[8000, 8000, 240000]</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -2972,7 +2803,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2987,65 +2818,67 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2137</v>
+        <v>2125</v>
       </c>
       <c r="H4" t="n">
-        <v>15000</v>
+        <v>48000</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3DSGS1G4000SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>M4G</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>2137</v>
+          <t>E210430011BYB</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2325</t>
+        </is>
       </c>
       <c r="M4" t="n">
-        <v>15000</v>
+        <v>48000</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>7500</v>
+        <v>3000</v>
       </c>
       <c r="P4" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>[0, 15000, 15000]</t>
+          <t>[48000, 48000, 60000]</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>[0, 1, 1]</t>
+          <t>[1, 1, 0]</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>[15000, 15000, 120000]</t>
+          <t>[48000, 48000, 240000]</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -3062,7 +2895,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3077,56 +2910,57 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>MBRD5100G-L10</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>F210813041AC</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2148</v>
+        <v>2125</v>
       </c>
       <c r="H5" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3DYMBRD5100SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>MBRD5100</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>F210813041AC</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>2148</v>
+          <t>E210430011BYB</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2325</t>
+        </is>
       </c>
       <c r="M5" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>LSYM
-MBRD5100</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="P5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>[5000, 5000, 50000]</t>
+          <t>[9000, 9000, 60000]</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -3136,7 +2970,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>[5000, 5000, 200000]</t>
+          <t>[9000, 9000, 240000]</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -3153,7 +2987,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3168,55 +3002,55 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2239</v>
+        <v>2251</v>
       </c>
       <c r="H6" t="n">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3DZ013W505S0B02</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>2239</v>
+        <v>2251</v>
       </c>
       <c r="M6" t="n">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="O6" t="n">
         <v>3000</v>
       </c>
       <c r="P6" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>[6000, 6000, 60000]</t>
+          <t>[36000, 36000, 60000]</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -3226,7 +3060,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[6000, 6000, 240000]</t>
+          <t>[36000, 36000, 240000]</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -3243,7 +3077,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3258,55 +3092,55 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>P2SD75AG-730</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2325</v>
+        <v>2251</v>
       </c>
       <c r="H7" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3DT075200U0SB01</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>P2SD75AG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>2325</v>
+        <v>2251</v>
       </c>
       <c r="M7" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>XR</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="P7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>[5000, 5000, 60000]</t>
+          <t>[3000, 3000, 60000]</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -3316,103 +3150,10 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>[5000, 5000, 240000]</t>
+          <t>[3000, 3000, 240000]</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024/03/13</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>I230815001</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>B0000010-3</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>協禧微機電</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG-L10</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>F210416513K3</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>2150</v>
-      </c>
-      <c r="H8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>3DT064400U0SB03</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>F210416513K3</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>2150</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>LSYM
-RM</t>
-        </is>
-      </c>
-      <c r="O8" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P8" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 25200]</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 100800]</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
         <is>
           <t>[1, 2, 0]</t>
         </is>
@@ -3429,7 +3170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3440,50 +3181,50 @@
     <col width="16" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="10" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>purchase_order</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>product_number</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>customer_part_number</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>new_lot</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>new_quantity</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>marking_code</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>sampling</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>DC</t>
         </is>
@@ -3492,255 +3233,217 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091240100179</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
+          <t>F210720012AEB</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3000</v>
+        <v>16000</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>125</v>
+        <v>315</v>
       </c>
       <c r="H2" t="n">
-        <v>2315</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091240200042</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1N4148WG</t>
+          <t>1SS388</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
+          <t>F22021001106</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>77000</v>
+        <v>8000</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="H3" t="n">
-        <v>2315</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091231200081</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>M4G</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3DSGS1G4000SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
+          <t>E210430011BYB</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>15000</v>
+        <v>48000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>315</v>
+        <v>500</v>
       </c>
       <c r="H4" t="n">
-        <v>2137</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PB1-2307000305</t>
+          <t>P0091231200126</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MBRD5100</t>
+          <t>GLS6206P-T3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3DYMBRD5100SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>F210813041AC</t>
+          <t>E210430011BYB</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>LSYM
-MBRD5100</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="G5" t="n">
         <v>200</v>
       </c>
       <c r="H5" t="n">
-        <v>2148</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PB1-2111000268</t>
+          <t>P0091240100028</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3DZ013W505S0B02</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="H6" t="n">
-        <v>2239</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PB1-2308000138</t>
+          <t>P0091240100063</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P2SD75AG</t>
+          <t>LS5019NG-T3R</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3DT075200U0SB01</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>XR</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="H7" t="n">
-        <v>2325</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PB1-2105000582</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>3DT064400U0SB03</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>F210416513K3</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>LSYM
-RM</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>200</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2150</v>
+        <v>2251</v>
       </c>
     </row>
   </sheetData>
@@ -3754,7 +3457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3764,75 +3467,75 @@
   <cols>
     <col width="16" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="16" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="9" customWidth="1" min="9" max="9"/>
     <col width="6" customWidth="1" min="10" max="10"/>
     <col width="7" customWidth="1" min="11" max="11"/>
     <col width="9" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>invoice_series</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>customer_name</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>part_number</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>lot</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>DC</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>customer_part_number</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>marking_code</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>package</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>MPQ</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>store</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>expired</t>
         </is>
@@ -3841,7 +3544,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3851,51 +3554,51 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
+          <t>F210720012AE</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2315</v>
+        <v>2146</v>
       </c>
       <c r="F2" t="n">
-        <v>3000</v>
+        <v>16000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>SOD123</t>
+          <t>SOD523</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>Z13</t>
         </is>
       </c>
       <c r="L2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3905,41 +3608,41 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1SS388G-L10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
+          <t>F22021001106</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2315</v>
+        <v>2210</v>
       </c>
       <c r="F3" t="n">
-        <v>77000</v>
+        <v>8000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3DS1N4148W0SB01</t>
+          <t>10D3-S388-7B01</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>SOD123</t>
+          <t>SOD523</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>暫</t>
         </is>
       </c>
       <c r="L3" t="b">
@@ -3949,7 +3652,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3959,51 +3662,51 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2137</v>
+        <v>2125</v>
       </c>
       <c r="F4" t="n">
-        <v>15000</v>
+        <v>48000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3DSGS1G4000SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>SMA</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>7500</v>
+        <v>3000</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>X1</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="L4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4013,52 +3716,51 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MBRD5100G-L10</t>
+          <t>GLS6206PG-T3-LS0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>F210813041AC</t>
+          <t>E210430011BY</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2148</v>
+        <v>2125</v>
       </c>
       <c r="F5" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3DYMBRD5100SB01</t>
+          <t>10T4-206P-2R01</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>LSYM
-MBRD5100</t>
+          <t>8P</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>TO252</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="L5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -4068,33 +3770,33 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2239</v>
+        <v>2251</v>
       </c>
       <c r="F6" t="n">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3DZ013W505S0B02</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>SOD123</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="J6" t="n">
@@ -4102,7 +3804,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="L6" t="b">
@@ -4112,7 +3814,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>I230815001</t>
+          <t>IS24031302</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4122,99 +3824,44 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>P2SD75AG-730</t>
+          <t>PS5020KN-CU-L10</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
+          <t>E221110011AX</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2325</v>
+        <v>2251</v>
       </c>
       <c r="F7" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3DT075200U0SB01</t>
+          <t>10T3-5019-2R01</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>XR</t>
+          <t>K38</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>SOD123FL</t>
+          <t>SOT23</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>I2</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="L7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>I230815001</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>協禧微機電</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG-L10</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>F210416513K3</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>2150</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>3DT064400U0SB03</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>LSYM
-RM</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>SMA</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>1800</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>A7</t>
-        </is>
-      </c>
-      <c r="L8" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix label calculation pring flow
</commit_message>
<xml_diff>
--- a/parameters_dataframe.xlsx
+++ b/parameters_dataframe.xlsx
@@ -2186,22 +2186,22 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>[3000, 3000, 60000]</t>
+          <t>[3000, 60000, 3000]</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>[3000, 3000, 240000]</t>
+          <t>[3000, 240000, 3000]</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA2" t="n">
@@ -2337,22 +2337,22 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>[6000, 6000, 60000]</t>
+          <t>[6000, 60000, 6000]</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>[6000, 6000, 240000]</t>
+          <t>[6000, 240000, 6000]</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA3" t="n">
@@ -2498,12 +2498,12 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>[15000, 15000, 120000]</t>
+          <t>[15000, 120000, 15000]</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA4" t="n">
@@ -2639,22 +2639,22 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>[0, 30000, 15000]</t>
+          <t>[0, 15000, 30000]</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>[0, 1, 2]</t>
+          <t>[0, 2, 1]</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>[30000, 30000, 120000]</t>
+          <t>[30000, 120000, 30000]</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA5" t="n">
@@ -2790,22 +2790,22 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>[5000, 35000, 15000]</t>
+          <t>[5000, 15000, 35000]</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>[1, 1, 2]</t>
+          <t>[1, 2, 1]</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>[35000, 35000, 120000]</t>
+          <t>[35000, 120000, 35000]</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA6" t="n">
@@ -2941,22 +2941,22 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>[2500, 2500, 15000]</t>
+          <t>[2500, 15000, 2500]</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>[2500, 2500, 120000]</t>
+          <t>[2500, 120000, 2500]</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA7" t="n">
@@ -3094,22 +3094,22 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>[6000, 6000, 60000]</t>
+          <t>[6000, 60000, 6000]</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>[6000, 6000, 240000]</t>
+          <t>[6000, 240000, 6000]</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA8" t="n">
@@ -3247,22 +3247,22 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>[6000, 6000, 60000]</t>
+          <t>[6000, 60000, 6000]</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>[6000, 6000, 240000]</t>
+          <t>[6000, 240000, 6000]</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA9" t="n">
@@ -3400,22 +3400,22 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>[12000, 12000, 60000]</t>
+          <t>[12000, 60000, 12000]</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>[12000, 12000, 240000]</t>
+          <t>[12000, 240000, 12000]</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA10" t="n">
@@ -3553,22 +3553,22 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>[18000, 18000, 60000]</t>
+          <t>[18000, 60000, 18000]</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>[18000, 18000, 240000]</t>
+          <t>[18000, 240000, 18000]</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA11" t="n">
@@ -3706,22 +3706,22 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>[15000, 15000, 60000]</t>
+          <t>[15000, 60000, 15000]</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>[15000, 15000, 240000]</t>
+          <t>[15000, 240000, 15000]</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA12" t="n">
@@ -3857,22 +3857,22 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>[12000, 12000, 60000]</t>
+          <t>[12000, 60000, 12000]</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>[12000, 12000, 240000]</t>
+          <t>[12000, 240000, 12000]</t>
         </is>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA13" t="n">
@@ -4008,22 +4008,22 @@
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>[15000, 15000, 60000]</t>
+          <t>[15000, 60000, 15000]</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>[15000, 15000, 240000]</t>
+          <t>[15000, 240000, 15000]</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA14" t="n">
@@ -4161,22 +4161,22 @@
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>[5000, 5000, 60000]</t>
+          <t>[5000, 60000, 5000]</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>[5000, 5000, 240000]</t>
+          <t>[5000, 240000, 5000]</t>
         </is>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA15" t="n">
@@ -4312,22 +4312,22 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>[5000, 5000, 60000]</t>
+          <t>[5000, 60000, 5000]</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>[5000, 5000, 240000]</t>
+          <t>[5000, 240000, 5000]</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA16" t="n">
@@ -4463,22 +4463,22 @@
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>[10000, 10000, 60000]</t>
+          <t>[10000, 60000, 10000]</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>[10000, 10000, 240000]</t>
+          <t>[10000, 240000, 10000]</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA17" t="n">
@@ -4615,22 +4615,22 @@
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>[1800, 1800, 25200]</t>
+          <t>[1800, 21600, 1800]</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>[1800, 1800, 100800]</t>
+          <t>[1800, 86400, 1800]</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA18" t="n">
@@ -4767,22 +4767,22 @@
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>[3600, 3600, 25200]</t>
+          <t>[3600, 21600, 3600]</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>[3600, 3600, 100800]</t>
+          <t>[3600, 86400, 3600]</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA19" t="n">
@@ -4919,22 +4919,22 @@
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>[3600, 3600, 25200]</t>
+          <t>[3600, 21600, 3600]</t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>[3600, 3600, 100800]</t>
+          <t>[3600, 86400, 3600]</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA20" t="n">
@@ -5071,22 +5071,22 @@
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>[7200, 7200, 25200]</t>
+          <t>[7200, 21600, 7200]</t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>[7200, 7200, 100800]</t>
+          <t>[7200, 86400, 7200]</t>
         </is>
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA21" t="n">
@@ -5223,22 +5223,22 @@
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>[9000, 9000, 25200]</t>
+          <t>[9000, 21600, 9000]</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>[9000, 9000, 100800]</t>
+          <t>[9000, 86400, 9000]</t>
         </is>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA22" t="n">
@@ -5375,22 +5375,22 @@
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>[3600, 3600, 25200]</t>
+          <t>[3600, 21600, 3600]</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>[3600, 3600, 100800]</t>
+          <t>[3600, 86400, 3600]</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA23" t="n">
@@ -5527,22 +5527,22 @@
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>[18000, 43200, 25200]</t>
+          <t>[0, 21600, 43200]</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[0, 2, 1]</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>[43200, 43200, 100800]</t>
+          <t>[43200, 86400, 43200]</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA24" t="n">
@@ -5674,22 +5674,22 @@
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t>[27000, 27000, 60000]</t>
+          <t>[27000, 60000, 27000]</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>[27000, 27000, 240000]</t>
+          <t>[27000, 240000, 27000]</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA25" t="n">
@@ -5821,22 +5821,22 @@
       </c>
       <c r="W26" t="inlineStr">
         <is>
-          <t>[42000, 42000, 60000]</t>
+          <t>[42000, 60000, 42000]</t>
         </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>[42000, 42000, 240000]</t>
+          <t>[42000, 240000, 42000]</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA26" t="n">
@@ -5974,22 +5974,22 @@
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>[3000, 3000, 60000]</t>
+          <t>[3000, 60000, 3000]</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>[3000, 3000, 240000]</t>
+          <t>[3000, 240000, 3000]</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA27" t="n">
@@ -6133,22 +6133,22 @@
       </c>
       <c r="W28" t="inlineStr">
         <is>
-          <t>[15000, 15000, 60000]</t>
+          <t>[15000, 60000, 15000]</t>
         </is>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
         <is>
-          <t>[15000, 15000, 240000]</t>
+          <t>[15000, 240000, 15000]</t>
         </is>
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA28" t="n">
@@ -6292,22 +6292,22 @@
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>[9000, 9000, 60000]</t>
+          <t>[9000, 60000, 9000]</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>[9000, 9000, 240000]</t>
+          <t>[9000, 240000, 9000]</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA29" t="n">
@@ -6450,22 +6450,22 @@
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>[7500, 7500, 15000]</t>
+          <t>[7500, 15000, 7500]</t>
         </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>[7500, 7500, 120000]</t>
+          <t>[7500, 120000, 7500]</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA30" t="n">
@@ -6602,22 +6602,22 @@
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>[7500, 7500, 15000]</t>
+          <t>[7500, 15000, 7500]</t>
         </is>
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>[7500, 7500, 120000]</t>
+          <t>[7500, 120000, 7500]</t>
         </is>
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA31" t="n">
@@ -6754,22 +6754,22 @@
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>[7500, 7500, 15000]</t>
+          <t>[7500, 15000, 7500]</t>
         </is>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>[7500, 7500, 120000]</t>
+          <t>[7500, 120000, 7500]</t>
         </is>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
       <c r="AA32" t="n">
@@ -9993,7 +9993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10001,125 +10001,89 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="6" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="19" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
     <col width="22" customWidth="1" min="9" max="9"/>
-    <col width="22" customWidth="1" min="10" max="10"/>
-    <col width="19" customWidth="1" min="11" max="11"/>
-    <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="14" customWidth="1" min="14" max="14"/>
-    <col width="22" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="23" customWidth="1" min="17" max="17"/>
-    <col width="21" customWidth="1" min="18" max="18"/>
-    <col width="24" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="23" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="12" max="12"/>
+    <col width="24" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="inlineStr">
         <is>
-          <t>delivery_date</t>
+          <t>customer_no</t>
         </is>
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>invoice_series</t>
+          <t>customer_name</t>
         </is>
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>customer_no</t>
+          <t>purchase_order</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>customer_name</t>
+          <t>customer_part_number</t>
         </is>
       </c>
       <c r="E1" s="4" t="inlineStr">
         <is>
-          <t>part_number</t>
+          <t>product_number</t>
         </is>
       </c>
       <c r="F1" s="4" t="inlineStr">
         <is>
-          <t>lot</t>
+          <t>new_lot</t>
         </is>
       </c>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>DC</t>
+          <t>new_DC</t>
         </is>
       </c>
       <c r="H1" s="4" t="inlineStr">
         <is>
-          <t>quantity</t>
+          <t>new_quantity</t>
         </is>
       </c>
       <c r="I1" s="4" t="inlineStr">
         <is>
-          <t>customer_part_number</t>
+          <t>small_label_quantity</t>
         </is>
       </c>
       <c r="J1" s="4" t="inlineStr">
         <is>
-          <t>product_number</t>
+          <t>small_label_copies</t>
         </is>
       </c>
       <c r="K1" s="4" t="inlineStr">
         <is>
-          <t>new_lot</t>
+          <t>medium_label_quantity</t>
         </is>
       </c>
       <c r="L1" s="4" t="inlineStr">
         <is>
-          <t>new_DC</t>
+          <t>medium_label_copies</t>
         </is>
       </c>
       <c r="M1" s="4" t="inlineStr">
         <is>
-          <t>new_quantity</t>
+          <t>large_label_quantity</t>
         </is>
       </c>
       <c r="N1" s="4" t="inlineStr">
-        <is>
-          <t>marking_code</t>
-        </is>
-      </c>
-      <c r="O1" s="4" t="inlineStr">
-        <is>
-          <t>small_label_quantity</t>
-        </is>
-      </c>
-      <c r="P1" s="4" t="inlineStr">
-        <is>
-          <t>small_label_copies</t>
-        </is>
-      </c>
-      <c r="Q1" s="4" t="inlineStr">
-        <is>
-          <t>medium_label_quantity</t>
-        </is>
-      </c>
-      <c r="R1" s="4" t="inlineStr">
-        <is>
-          <t>medium_label_copies</t>
-        </is>
-      </c>
-      <c r="S1" s="4" t="inlineStr">
-        <is>
-          <t>large_label_quantity</t>
-        </is>
-      </c>
-      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>large_label_copies</t>
         </is>
@@ -10128,27 +10092,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2402000054</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DS1N4148W0SB01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1N4148WG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -10162,83 +10126,57 @@
       <c r="H2" t="n">
         <v>3000</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>3DS1N4148W0SB01</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>1N4148WG</t>
-        </is>
+      <c r="I2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>F230316011EH</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>2315</v>
-      </c>
-      <c r="M2" t="n">
-        <v>3000</v>
+          <t>[3000, 60000, 3000]</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>[3000, 240000, 3000]</t>
+        </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>T4</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>[3000, 3000, 60000]</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>[3000, 3000, 240000]</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2402000054</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DS1N4148W0SB01</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1N4148WG-Cu-L10</t>
+          <t>1N4148WG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -10252,83 +10190,57 @@
       <c r="H3" t="n">
         <v>6000</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3DS1N4148W0SB01</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1N4148WG</t>
-        </is>
+      <c r="I3" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>F23031601109</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>2315</v>
-      </c>
-      <c r="M3" t="n">
-        <v>6000</v>
+          <t>[6000, 60000, 6000]</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>[6000, 240000, 6000]</t>
+        </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>T4</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>[6000, 6000, 60000]</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>[6000, 6000, 240000]</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000055</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DSGS1G4000SB01</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>M4G</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -10342,83 +10254,57 @@
       <c r="H4" t="n">
         <v>15000</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3DSGS1G4000SB01</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>M4G</t>
-        </is>
+      <c r="I4" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>2137</v>
-      </c>
-      <c r="M4" t="n">
-        <v>15000</v>
+          <t>[0, 15000, 15000]</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>[0, 1, 1]</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>[15000, 120000, 15000]</t>
+        </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
-        </is>
-      </c>
-      <c r="O4" t="n">
-        <v>7500</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>[0, 15000, 15000]</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>[0, 1, 1]</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>[15000, 15000, 120000]</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000153</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DSGS1G4000SB01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>M4G</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -10432,83 +10318,57 @@
       <c r="H5" t="n">
         <v>30000</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>3DSGS1G4000SB01</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>M4G</t>
-        </is>
+      <c r="I5" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>2137</v>
-      </c>
-      <c r="M5" t="n">
-        <v>30000</v>
+          <t>[0, 15000, 30000]</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>[0, 2, 1]</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>[30000, 120000, 30000]</t>
+        </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
-        </is>
-      </c>
-      <c r="O5" t="n">
-        <v>7500</v>
-      </c>
-      <c r="P5" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>[0, 30000, 15000]</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>[0, 1, 2]</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>[30000, 30000, 120000]</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000112</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DSGS1G4000SB01</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>M4G</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -10522,83 +10382,57 @@
       <c r="H6" t="n">
         <v>35000</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>3DSGS1G4000SB01</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>M4G</t>
-        </is>
+      <c r="I6" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>2137</v>
-      </c>
-      <c r="M6" t="n">
-        <v>35000</v>
+          <t>[5000, 15000, 35000]</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>[1, 2, 1]</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>[35000, 120000, 35000]</t>
+        </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
-        </is>
-      </c>
-      <c r="O6" t="n">
-        <v>7500</v>
-      </c>
-      <c r="P6" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>[5000, 35000, 15000]</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>[1, 1, 2]</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>[35000, 35000, 120000]</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000114</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DSGS1G4000SB01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>M4G-100</t>
+          <t>M4G</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -10612,543 +10446,387 @@
       <c r="H7" t="n">
         <v>2500</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>3DSGS1G4000SB01</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>M4G</t>
-        </is>
+      <c r="I7" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>ZR374H600Z0710</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>2137</v>
-      </c>
-      <c r="M7" t="n">
-        <v>2500</v>
+          <t>[2500, 15000, 2500]</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>[2500, 120000, 2500]</t>
+        </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>LSYM M4</t>
-        </is>
-      </c>
-      <c r="O7" t="n">
-        <v>7500</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>[2500, 2500, 15000]</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>[2500, 2500, 120000]</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000050</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3TSNMMST4401B01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>MMST4401G-3T3R-L10</t>
+          <t>MMST4401G</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>F21050551107</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>2143</v>
+          <t>F21050551107B</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2343</t>
+        </is>
       </c>
       <c r="H8" t="n">
         <v>6000</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>3TSNMMST4401B01</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>MMST4401G</t>
-        </is>
+      <c r="I8" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>F21050551107B</t>
+          <t>[6000, 60000, 6000]</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2343</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>6000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>[6000, 240000, 6000]</t>
+        </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>K3X</t>
-        </is>
-      </c>
-      <c r="O8" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P8" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>[6000, 6000, 60000]</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>[6000, 6000, 240000]</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000092</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3TSNMMST4401B01</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>MMST4401G-3T3R-L10</t>
+          <t>MMST4401G</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>F21050551107</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>2143</v>
+          <t>F21050551107B</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2343</t>
+        </is>
       </c>
       <c r="H9" t="n">
         <v>6000</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>3TSNMMST4401B01</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>MMST4401G</t>
-        </is>
+      <c r="I9" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>F21050551107B</t>
+          <t>[6000, 60000, 6000]</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2343</t>
-        </is>
-      </c>
-      <c r="M9" t="n">
-        <v>6000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>[6000, 240000, 6000]</t>
+        </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>K3X</t>
-        </is>
-      </c>
-      <c r="O9" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P9" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>[6000, 6000, 60000]</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>[6000, 6000, 240000]</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2312000284</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DZ013W505S0B02</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>MMSZ5243BG銀河品牌</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>2239</v>
+          <t>F220322022DKA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2339</t>
+        </is>
       </c>
       <c r="H10" t="n">
         <v>12000</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>3DZ013W505S0B02</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>MMSZ5243BG銀河品牌</t>
-        </is>
+      <c r="I10" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>F220322022DKA</t>
+          <t>[12000, 60000, 12000]</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2339</t>
-        </is>
-      </c>
-      <c r="M10" t="n">
-        <v>12000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>[12000, 240000, 12000]</t>
+        </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>H3</t>
-        </is>
-      </c>
-      <c r="O10" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P10" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>[12000, 12000, 60000]</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>[12000, 12000, 240000]</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000153</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DZ013W505S0B02</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>MMSZ5243BG銀河品牌</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>F220322022DK</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>2239</v>
+          <t>F220322022DKA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2339</t>
+        </is>
       </c>
       <c r="H11" t="n">
         <v>18000</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>3DZ013W505S0B02</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>MMSZ5243BG銀河品牌</t>
-        </is>
+      <c r="I11" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J11" t="n">
+        <v>6</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>F220322022DKA</t>
+          <t>[18000, 60000, 18000]</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2339</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
-        <v>18000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>[18000, 240000, 18000]</t>
+        </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>H3</t>
-        </is>
-      </c>
-      <c r="O11" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P11" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>[18000, 18000, 60000]</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>[18000, 18000, 240000]</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000153</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DZ013W505S0B02</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>MMSZ5243BG-L10</t>
+          <t>MMSZ5243BG銀河品牌</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>F220926011A5</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>2243</v>
+          <t>F220926011A5A</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2343</t>
+        </is>
       </c>
       <c r="H12" t="n">
         <v>15000</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3DZ013W505S0B02</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>MMSZ5243BG銀河品牌</t>
-        </is>
+      <c r="I12" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>F220926011A5A</t>
+          <t>[15000, 60000, 15000]</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2343</t>
-        </is>
-      </c>
-      <c r="M12" t="n">
-        <v>15000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>[15000, 240000, 15000]</t>
+        </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>H3</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P12" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>[15000, 15000, 60000]</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>[15000, 15000, 240000]</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000283</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DZ036W505S0B01</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>MMSZ5258BG-L10</t>
+          <t>MMSZ5258BG(銀河品牌)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -11162,83 +10840,57 @@
       <c r="H13" t="n">
         <v>12000</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>3DZ036W505S0B01</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>MMSZ5258BG(銀河品牌)</t>
-        </is>
+      <c r="I13" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J13" t="n">
+        <v>4</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>F230413022D7</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>2319</v>
-      </c>
-      <c r="M13" t="n">
-        <v>12000</v>
+          <t>[12000, 60000, 12000]</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>[12000, 240000, 12000]</t>
+        </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="O13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P13" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>[12000, 12000, 60000]</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>[12000, 12000, 240000]</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2402000054</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT026200U0SB01</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>P2SD26AG-730</t>
+          <t>P2SD26AG</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -11252,175 +10904,123 @@
       <c r="H14" t="n">
         <v>15000</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>3DT026200U0SB01</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>P2SD26AG</t>
-        </is>
+      <c r="I14" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J14" t="n">
+        <v>6</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>H3042811001</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>2317</v>
-      </c>
-      <c r="M14" t="n">
-        <v>15000</v>
+          <t>[15000, 60000, 15000]</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>[15000, 240000, 15000]</t>
+        </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>CE</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>2500</v>
-      </c>
-      <c r="P14" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>[15000, 15000, 60000]</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>[15000, 15000, 240000]</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000111</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT048200U0SB01</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>P2SD48AG-730</t>
+          <t>P2SD48AG</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>H202102041101006</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>2106</v>
+          <t>H202102041101006C</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2406</t>
+        </is>
       </c>
       <c r="H15" t="n">
         <v>5000</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>3DT048200U0SB01</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>P2SD48AG</t>
-        </is>
+      <c r="I15" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>H202102041101006C</t>
+          <t>[5000, 60000, 5000]</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2406</t>
-        </is>
-      </c>
-      <c r="M15" t="n">
-        <v>5000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>[5000, 240000, 5000]</t>
+        </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>CX</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>2500</v>
-      </c>
-      <c r="P15" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>[5000, 5000, 60000]</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>[5000, 5000, 240000]</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000153</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT075200U0SB01</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>P2SD75AG-730</t>
+          <t>P2SD75AG</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -11434,83 +11034,57 @@
       <c r="H16" t="n">
         <v>5000</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3DT075200U0SB01</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>P2SD75AG</t>
-        </is>
+      <c r="I16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>2325</v>
-      </c>
-      <c r="M16" t="n">
-        <v>5000</v>
+          <t>[5000, 60000, 5000]</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>[5000, 240000, 5000]</t>
+        </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>XR</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>2500</v>
-      </c>
-      <c r="P16" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>[5000, 5000, 60000]</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>[5000, 5000, 240000]</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2402000054</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT075200U0SB01</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>P2SD75AG-730</t>
+          <t>P2SD75AG</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -11524,83 +11098,57 @@
       <c r="H17" t="n">
         <v>10000</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>3DT075200U0SB01</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>P2SD75AG</t>
-        </is>
+      <c r="I17" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>H202306201101002</t>
-        </is>
-      </c>
-      <c r="L17" t="n">
-        <v>2325</v>
-      </c>
-      <c r="M17" t="n">
-        <v>10000</v>
+          <t>[10000, 60000, 10000]</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>[10000, 240000, 10000]</t>
+        </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>XR</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>2500</v>
-      </c>
-      <c r="P17" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>[10000, 10000, 60000]</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>[10000, 10000, 240000]</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2312000284</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT040400U0SB04</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>P4SMAJ40AG-L10</t>
+          <t>P4SMAJ40AG</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -11614,84 +11162,57 @@
       <c r="H18" t="n">
         <v>1800</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>3DT040400U0SB04</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>P4SMAJ40AG</t>
-        </is>
+      <c r="I18" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>F230306522RJ</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>2311</v>
-      </c>
-      <c r="M18" t="n">
-        <v>1800</v>
+          <t>[1800, 21600, 1800]</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>[1800, 86400, 1800]</t>
+        </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>LSYM
-CR</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>[1800, 1800, 25200]</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>[1800, 1800, 100800]</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2312000284</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT040400U0SB04</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>P4SMAJ40AG-L10</t>
+          <t>P4SMAJ40AG</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -11705,84 +11226,57 @@
       <c r="H19" t="n">
         <v>3600</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>3DT040400U0SB04</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>P4SMAJ40AG</t>
-        </is>
+      <c r="I19" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>F2303175220V</t>
-        </is>
-      </c>
-      <c r="L19" t="n">
-        <v>2312</v>
-      </c>
-      <c r="M19" t="n">
-        <v>3600</v>
+          <t>[3600, 21600, 3600]</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>[3600, 86400, 3600]</t>
+        </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>LSYM
-CR</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P19" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 25200]</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 100800]</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000153</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT040400U0SB04</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>P4SMAJ40AG-L10</t>
+          <t>P4SMAJ40AG</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -11796,84 +11290,57 @@
       <c r="H20" t="n">
         <v>3600</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3DT040400U0SB04</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>P4SMAJ40AG</t>
-        </is>
+      <c r="I20" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>F2303175220V</t>
-        </is>
-      </c>
-      <c r="L20" t="n">
-        <v>2312</v>
-      </c>
-      <c r="M20" t="n">
-        <v>3600</v>
+          <t>[3600, 21600, 3600]</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>[3600, 86400, 3600]</t>
+        </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>LSYM
-CR</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P20" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 25200]</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 100800]</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000153</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT040400U0SB04</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>P4SMAJ40AG-L10</t>
+          <t>P4SMAJ40AG</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -11887,84 +11354,57 @@
       <c r="H21" t="n">
         <v>7200</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>3DT040400U0SB04</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>P4SMAJ40AG</t>
-        </is>
+      <c r="I21" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>F230327512KV</t>
-        </is>
-      </c>
-      <c r="L21" t="n">
-        <v>2317</v>
-      </c>
-      <c r="M21" t="n">
-        <v>7200</v>
+          <t>[7200, 21600, 7200]</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>[7200, 86400, 7200]</t>
+        </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>LSYM
-CR</t>
-        </is>
-      </c>
-      <c r="O21" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P21" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>[7200, 7200, 25200]</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>[7200, 7200, 100800]</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000283</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT040400U0SB04</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>P4SMAJ40AG-L10</t>
+          <t>P4SMAJ40AG</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -11978,84 +11418,57 @@
       <c r="H22" t="n">
         <v>9000</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>3DT040400U0SB04</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>P4SMAJ40AG</t>
-        </is>
+      <c r="I22" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J22" t="n">
+        <v>5</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>F230327512KV</t>
-        </is>
-      </c>
-      <c r="L22" t="n">
-        <v>2317</v>
-      </c>
-      <c r="M22" t="n">
-        <v>9000</v>
+          <t>[9000, 21600, 9000]</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>[9000, 86400, 9000]</t>
+        </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>LSYM
-CR</t>
-        </is>
-      </c>
-      <c r="O22" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P22" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>[9000, 9000, 25200]</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>[9000, 9000, 100800]</t>
-        </is>
-      </c>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000050</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT043400U0SB04</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>P4SMAJ43AG-L10</t>
+          <t>P4SMAJ43AG</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -12069,84 +11482,57 @@
       <c r="H23" t="n">
         <v>3600</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>3DT043400U0SB04</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>P4SMAJ43AG</t>
-        </is>
+      <c r="I23" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J23" t="n">
+        <v>2</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>X200415011AR</t>
-        </is>
-      </c>
-      <c r="L23" t="n">
-        <v>2021</v>
-      </c>
-      <c r="M23" t="n">
-        <v>3600</v>
+          <t>[3600, 21600, 3600]</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>[3600, 86400, 3600]</t>
+        </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>LSYM
-CT</t>
-        </is>
-      </c>
-      <c r="O23" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P23" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 25200]</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>[3600, 3600, 100800]</t>
-        </is>
-      </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000112</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DT064400U0SB03</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>P4SMAJ64AG-730</t>
+          <t>P4SMAJ64AG</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -12160,84 +11546,57 @@
       <c r="H24" t="n">
         <v>43200</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>3DT064400U0SB03</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>P4SMAJ64AG</t>
-        </is>
+      <c r="I24" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J24" t="n">
+        <v>24</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>H202108101101001</t>
-        </is>
-      </c>
-      <c r="L24" t="n">
-        <v>2136</v>
-      </c>
-      <c r="M24" t="n">
-        <v>43200</v>
+          <t>[0, 21600, 43200]</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>[0, 2, 1]</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>[43200, 86400, 43200]</t>
+        </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>LSYM
-RM</t>
-        </is>
-      </c>
-      <c r="O24" t="n">
-        <v>1800</v>
-      </c>
-      <c r="P24" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>[18000, 43200, 25200]</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>[1, 1, 1]</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>[43200, 43200, 100800]</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2312000190</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DSGS1006FLSB01</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>S10MHG-1-060</t>
+          <t>S10JHG</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -12249,81 +11608,57 @@
       <c r="H25" t="n">
         <v>27000</v>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>3DSGS1006FLSB01</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>S10JHG</t>
-        </is>
-      </c>
-      <c r="K25" t="n">
-        <v>34331004</v>
-      </c>
-      <c r="L25" t="n">
-        <v>2314</v>
-      </c>
-      <c r="M25" t="n">
-        <v>27000</v>
+      <c r="I25" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J25" t="n">
+        <v>9</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>[27000, 60000, 27000]</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>[27000, 240000, 27000]</t>
+        </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>A7</t>
-        </is>
-      </c>
-      <c r="O25" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P25" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>[27000, 27000, 60000]</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>[27000, 27000, 240000]</t>
-        </is>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2312000284</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DSS10JHG00SB01</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>S10MHG-1-060</t>
+          <t>S10JHG</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -12335,357 +11670,255 @@
       <c r="H26" t="n">
         <v>42000</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>3DSS10JHG00SB01</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>S10JHG</t>
-        </is>
-      </c>
-      <c r="K26" t="n">
-        <v>34331004</v>
-      </c>
-      <c r="L26" t="n">
-        <v>2314</v>
-      </c>
-      <c r="M26" t="n">
-        <v>42000</v>
+      <c r="I26" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J26" t="n">
+        <v>14</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>[42000, 60000, 42000]</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>[42000, 240000, 42000]</t>
+        </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>A7</t>
-        </is>
-      </c>
-      <c r="O26" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P26" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>[42000, 42000, 60000]</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>[42000, 42000, 240000]</t>
-        </is>
-      </c>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2312000284</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DYSS104000SB01</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>SS1040G-CU-L10</t>
+          <t>SS1040G</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>E210907031C5</t>
-        </is>
-      </c>
-      <c r="G27" t="n">
-        <v>2148</v>
+          <t>E210907031C5B</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2348</t>
+        </is>
       </c>
       <c r="H27" t="n">
         <v>3000</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>3DYSS104000SB01</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>SS1040G</t>
-        </is>
+      <c r="I27" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>E210907031C5B</t>
+          <t>[3000, 60000, 3000]</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2348</t>
-        </is>
-      </c>
-      <c r="M27" t="n">
-        <v>3000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>[3000, 240000, 3000]</t>
+        </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>SL</t>
-        </is>
-      </c>
-      <c r="O27" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P27" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>[3000, 3000, 60000]</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>[3000, 3000, 240000]</t>
-        </is>
-      </c>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000055</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DYSS104000SB01</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>SS1040G-CU-L10</t>
+          <t>SS1040G</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>E210907031C5</t>
-        </is>
-      </c>
-      <c r="G28" t="n">
-        <v>2148</v>
+          <t>E210907031C5B</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2348</t>
+        </is>
       </c>
       <c r="H28" t="n">
         <v>15000</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>3DYSS104000SB01</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>SS1040G</t>
-        </is>
+      <c r="I28" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J28" t="n">
+        <v>5</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>E210907031C5B</t>
+          <t>[15000, 60000, 15000]</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2348</t>
-        </is>
-      </c>
-      <c r="M28" t="n">
-        <v>15000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>[15000, 240000, 15000]</t>
+        </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>SL</t>
-        </is>
-      </c>
-      <c r="O28" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P28" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>[15000, 15000, 60000]</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>[15000, 15000, 240000]</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2401000283</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DYSS104000SB01</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>SS1040G-CU-L10</t>
+          <t>SS1040G</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>E210907031C5</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
-        <v>2148</v>
+          <t>E210907031C5B</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2348</t>
+        </is>
       </c>
       <c r="H29" t="n">
         <v>9000</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>3DYSS104000SB01</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>SS1040G</t>
-        </is>
+      <c r="I29" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>E210907031C5B</t>
+          <t>[9000, 60000, 9000]</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2348</t>
-        </is>
-      </c>
-      <c r="M29" t="n">
-        <v>9000</v>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>[9000, 240000, 9000]</t>
+        </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>SL</t>
-        </is>
-      </c>
-      <c r="O29" t="n">
-        <v>3000</v>
-      </c>
-      <c r="P29" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>[9000, 9000, 60000]</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>[9000, 9000, 240000]</t>
-        </is>
-      </c>
-      <c r="T29" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2402000054</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DYSS34AG00SB01</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>SS34AG-L10</t>
+          <t>SS34AG</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -12699,84 +11932,57 @@
       <c r="H30" t="n">
         <v>7500</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>3DYSS34AG00SB01</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>SS34AG</t>
-        </is>
+      <c r="I30" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>F221129012GY</t>
-        </is>
-      </c>
-      <c r="L30" t="n">
-        <v>2302</v>
-      </c>
-      <c r="M30" t="n">
-        <v>7500</v>
+          <t>[7500, 15000, 7500]</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>[7500, 120000, 7500]</t>
+        </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>LSYM
-SS34A</t>
-        </is>
-      </c>
-      <c r="O30" t="n">
-        <v>7500</v>
-      </c>
-      <c r="P30" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>[7500, 7500, 15000]</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>[7500, 7500, 120000]</t>
-        </is>
-      </c>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2402000160</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DYSS34AG00SB01</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>SS34AG-L10</t>
+          <t>SS34AG</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -12790,84 +11996,57 @@
       <c r="H31" t="n">
         <v>7500</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>3DYSS34AG00SB01</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>SS34AG</t>
-        </is>
+      <c r="I31" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>F221129012GY</t>
-        </is>
-      </c>
-      <c r="L31" t="n">
-        <v>2302</v>
-      </c>
-      <c r="M31" t="n">
-        <v>7500</v>
+          <t>[7500, 15000, 7500]</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>[7500, 120000, 7500]</t>
+        </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>LSYM
-SS34A</t>
-        </is>
-      </c>
-      <c r="O31" t="n">
-        <v>7500</v>
-      </c>
-      <c r="P31" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>[7500, 7500, 15000]</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>[7500, 7500, 120000]</t>
-        </is>
-      </c>
-      <c r="T31" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2024/03/13</t>
+          <t>B0000010-3</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>I240319001</t>
+          <t>協禧微機電</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>B0000010-3</t>
+          <t>PB1-2403000090</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>協禧微機電</t>
+          <t>3DYSS34AG00SB01</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>SS34AG-L10</t>
+          <t>SS34AG</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -12881,57 +12060,30 @@
       <c r="H32" t="n">
         <v>7500</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>3DYSS34AG00SB01</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>SS34AG</t>
-        </is>
+      <c r="I32" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>F221129012GY</t>
-        </is>
-      </c>
-      <c r="L32" t="n">
-        <v>2302</v>
-      </c>
-      <c r="M32" t="n">
-        <v>7500</v>
+          <t>[7500, 15000, 7500]</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>[1, 0, 1]</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>[7500, 120000, 7500]</t>
+        </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>LSYM
-SS34A</t>
-        </is>
-      </c>
-      <c r="O32" t="n">
-        <v>7500</v>
-      </c>
-      <c r="P32" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>[7500, 7500, 15000]</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>[1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>[7500, 7500, 120000]</t>
-        </is>
-      </c>
-      <c r="T32" t="inlineStr">
-        <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 2]</t>
         </is>
       </c>
     </row>

</xml_diff>